<commit_message>
simulation seems fully continuous in nature now, except for discrete jumps between coefficients. I am implementing an interpolation tool for smooth transition between discrete values
</commit_message>
<xml_diff>
--- a/Aero design/Flight sim/hover stage sim - RK4 method/lookupTableCd.xlsx
+++ b/Aero design/Flight sim/hover stage sim - RK4 method/lookupTableCd.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joseph\Documents\Crash-Sat\Crash-Sat\Aero design\Flight sim\hover stage sim - RK4 method\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FAA0139-21F9-47DA-840B-E483F741334C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83096A00-A8AB-4AB5-B438-DDFA2E5A1C14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="900" yWindow="2640" windowWidth="17280" windowHeight="8976" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -351,108 +351,87 @@
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="J1" sqref="J1:K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1">
-        <v>8.0000000000000002E-3</v>
+        <v>1.6E-2</v>
       </c>
       <c r="B1">
-        <f>A1+0.002</f>
-        <v>0.01</v>
+        <v>1.6E-2</v>
       </c>
       <c r="C1">
-        <f t="shared" ref="C1:H1" si="0">B1+0.002</f>
-        <v>1.2E-2</v>
+        <v>1.6E-2</v>
       </c>
       <c r="D1">
-        <f t="shared" si="0"/>
-        <v>1.4E-2</v>
+        <v>1.6E-2</v>
       </c>
       <c r="E1">
-        <f t="shared" si="0"/>
         <v>1.6E-2</v>
       </c>
       <c r="F1">
-        <f t="shared" si="0"/>
-        <v>1.8000000000000002E-2</v>
+        <v>1.6E-2</v>
       </c>
       <c r="G1">
-        <f t="shared" si="0"/>
-        <v>2.0000000000000004E-2</v>
+        <v>1.6E-2</v>
       </c>
       <c r="H1">
-        <f t="shared" si="0"/>
-        <v>2.2000000000000006E-2</v>
+        <v>1.6E-2</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>4.0000000000000001E-3</v>
+        <v>9.0000000000000011E-3</v>
       </c>
       <c r="B2">
-        <f t="shared" ref="B2:H14" si="1">A2+0.002</f>
-        <v>6.0000000000000001E-3</v>
+        <v>9.0000000000000011E-3</v>
       </c>
       <c r="C2">
-        <f t="shared" si="1"/>
-        <v>8.0000000000000002E-3</v>
+        <v>9.0000000000000011E-3</v>
       </c>
       <c r="D2">
-        <f t="shared" si="1"/>
-        <v>0.01</v>
+        <v>9.0000000000000011E-3</v>
       </c>
       <c r="E2">
-        <f t="shared" si="1"/>
-        <v>1.2E-2</v>
+        <v>9.0000000000000011E-3</v>
       </c>
       <c r="F2">
-        <f t="shared" si="1"/>
-        <v>1.4E-2</v>
+        <v>9.0000000000000011E-3</v>
       </c>
       <c r="G2">
-        <f t="shared" si="1"/>
-        <v>1.6E-2</v>
+        <v>9.0000000000000011E-3</v>
       </c>
       <c r="H2">
-        <f t="shared" si="1"/>
-        <v>1.8000000000000002E-2</v>
+        <v>9.0000000000000011E-3</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>2E-3</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="B3">
-        <f t="shared" si="1"/>
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="C3">
-        <f t="shared" si="1"/>
-        <v>6.0000000000000001E-3</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="D3">
-        <f t="shared" si="1"/>
-        <v>8.0000000000000002E-3</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="E3">
-        <f t="shared" si="1"/>
-        <v>0.01</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="F3">
-        <f t="shared" si="1"/>
-        <v>1.2E-2</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="G3">
-        <f t="shared" si="1"/>
-        <v>1.4E-2</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="H3">
-        <f t="shared" si="1"/>
-        <v>1.6E-2</v>
+        <v>4.0000000000000001E-3</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
@@ -460,32 +439,25 @@
         <v>1E-3</v>
       </c>
       <c r="B4">
-        <f t="shared" si="1"/>
-        <v>3.0000000000000001E-3</v>
+        <v>1E-3</v>
       </c>
       <c r="C4">
-        <f t="shared" si="1"/>
-        <v>5.0000000000000001E-3</v>
+        <v>1E-3</v>
       </c>
       <c r="D4">
-        <f t="shared" si="1"/>
-        <v>7.0000000000000001E-3</v>
+        <v>1E-3</v>
       </c>
       <c r="E4">
-        <f t="shared" si="1"/>
-        <v>9.0000000000000011E-3</v>
+        <v>1E-3</v>
       </c>
       <c r="F4">
-        <f t="shared" si="1"/>
-        <v>1.1000000000000001E-2</v>
+        <v>1E-3</v>
       </c>
       <c r="G4">
-        <f t="shared" si="1"/>
-        <v>1.3000000000000001E-2</v>
+        <v>1E-3</v>
       </c>
       <c r="H4">
-        <f t="shared" si="1"/>
-        <v>1.5000000000000001E-2</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
@@ -493,32 +465,25 @@
         <v>0</v>
       </c>
       <c r="B5">
-        <f t="shared" si="1"/>
-        <v>2E-3</v>
+        <v>0</v>
       </c>
       <c r="C5">
-        <f t="shared" si="1"/>
-        <v>4.0000000000000001E-3</v>
+        <v>0</v>
       </c>
       <c r="D5">
-        <f t="shared" si="1"/>
-        <v>6.0000000000000001E-3</v>
+        <v>0</v>
       </c>
       <c r="E5">
-        <f t="shared" si="1"/>
-        <v>8.0000000000000002E-3</v>
+        <v>0</v>
       </c>
       <c r="F5">
-        <f t="shared" si="1"/>
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="G5">
-        <f t="shared" si="1"/>
-        <v>1.2E-2</v>
+        <v>0</v>
       </c>
       <c r="H5">
-        <f t="shared" si="1"/>
-        <v>1.4E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
@@ -526,296 +491,233 @@
         <v>1E-3</v>
       </c>
       <c r="B6">
-        <f t="shared" si="1"/>
-        <v>3.0000000000000001E-3</v>
+        <v>1E-3</v>
       </c>
       <c r="C6">
-        <f t="shared" si="1"/>
-        <v>5.0000000000000001E-3</v>
+        <v>1E-3</v>
       </c>
       <c r="D6">
-        <f t="shared" si="1"/>
-        <v>7.0000000000000001E-3</v>
+        <v>1E-3</v>
       </c>
       <c r="E6">
-        <f t="shared" si="1"/>
-        <v>9.0000000000000011E-3</v>
+        <v>1E-3</v>
       </c>
       <c r="F6">
-        <f t="shared" si="1"/>
-        <v>1.1000000000000001E-2</v>
+        <v>1E-3</v>
       </c>
       <c r="G6">
-        <f t="shared" si="1"/>
-        <v>1.3000000000000001E-2</v>
+        <v>1E-3</v>
       </c>
       <c r="H6">
-        <f t="shared" si="1"/>
-        <v>1.5000000000000001E-2</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>2E-3</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="B7">
-        <f t="shared" si="1"/>
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="C7">
-        <f t="shared" si="1"/>
-        <v>6.0000000000000001E-3</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="D7">
-        <f t="shared" si="1"/>
-        <v>8.0000000000000002E-3</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="E7">
-        <f t="shared" si="1"/>
-        <v>0.01</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="F7">
-        <f t="shared" si="1"/>
-        <v>1.2E-2</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="G7">
-        <f t="shared" si="1"/>
-        <v>1.4E-2</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="H7">
-        <f t="shared" si="1"/>
-        <v>1.6E-2</v>
+        <v>4.0000000000000001E-3</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8">
-        <v>4.0000000000000001E-3</v>
+        <v>9.0000000000000011E-3</v>
       </c>
       <c r="B8">
-        <f t="shared" si="1"/>
-        <v>6.0000000000000001E-3</v>
+        <v>9.0000000000000011E-3</v>
       </c>
       <c r="C8">
-        <f t="shared" si="1"/>
-        <v>8.0000000000000002E-3</v>
+        <v>9.0000000000000011E-3</v>
       </c>
       <c r="D8">
-        <f t="shared" si="1"/>
-        <v>0.01</v>
+        <v>9.0000000000000011E-3</v>
       </c>
       <c r="E8">
-        <f t="shared" si="1"/>
-        <v>1.2E-2</v>
+        <v>9.0000000000000011E-3</v>
       </c>
       <c r="F8">
-        <f t="shared" si="1"/>
-        <v>1.4E-2</v>
+        <v>9.0000000000000011E-3</v>
       </c>
       <c r="G8">
-        <f t="shared" si="1"/>
-        <v>1.6E-2</v>
+        <v>9.0000000000000011E-3</v>
       </c>
       <c r="H8">
-        <f t="shared" si="1"/>
-        <v>1.8000000000000002E-2</v>
+        <v>9.0000000000000011E-3</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9">
-        <v>8.0000000000000002E-3</v>
+        <v>1.6E-2</v>
       </c>
       <c r="B9">
-        <f t="shared" si="1"/>
-        <v>0.01</v>
+        <v>1.6E-2</v>
       </c>
       <c r="C9">
-        <f t="shared" si="1"/>
-        <v>1.2E-2</v>
+        <v>1.6E-2</v>
       </c>
       <c r="D9">
-        <f t="shared" si="1"/>
-        <v>1.4E-2</v>
+        <v>1.6E-2</v>
       </c>
       <c r="E9">
-        <f t="shared" si="1"/>
         <v>1.6E-2</v>
       </c>
       <c r="F9">
-        <f t="shared" si="1"/>
-        <v>1.8000000000000002E-2</v>
+        <v>1.6E-2</v>
       </c>
       <c r="G9">
-        <f t="shared" si="1"/>
-        <v>2.0000000000000004E-2</v>
+        <v>1.6E-2</v>
       </c>
       <c r="H9">
-        <f t="shared" si="1"/>
-        <v>2.2000000000000006E-2</v>
+        <v>1.6E-2</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10">
-        <v>1.6E-2</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="B10">
-        <f t="shared" si="1"/>
-        <v>1.8000000000000002E-2</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="C10">
-        <f t="shared" si="1"/>
-        <v>2.0000000000000004E-2</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="D10">
-        <f t="shared" si="1"/>
-        <v>2.2000000000000006E-2</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="E10">
-        <f t="shared" si="1"/>
-        <v>2.4000000000000007E-2</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="F10">
-        <f t="shared" si="1"/>
-        <v>2.6000000000000009E-2</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="G10">
-        <f t="shared" si="1"/>
-        <v>2.8000000000000011E-2</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="H10">
-        <f t="shared" si="1"/>
-        <v>3.0000000000000013E-2</v>
+        <v>2.5000000000000001E-2</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11">
-        <v>3.2000000000000001E-2</v>
+        <v>3.6000000000000004E-2</v>
       </c>
       <c r="B11">
-        <f t="shared" si="1"/>
-        <v>3.4000000000000002E-2</v>
+        <v>3.6000000000000004E-2</v>
       </c>
       <c r="C11">
-        <f t="shared" si="1"/>
         <v>3.6000000000000004E-2</v>
       </c>
       <c r="D11">
-        <f t="shared" si="1"/>
-        <v>3.8000000000000006E-2</v>
+        <v>3.6000000000000004E-2</v>
       </c>
       <c r="E11">
-        <f t="shared" si="1"/>
-        <v>4.0000000000000008E-2</v>
+        <v>3.6000000000000004E-2</v>
       </c>
       <c r="F11">
-        <f t="shared" si="1"/>
-        <v>4.200000000000001E-2</v>
+        <v>3.6000000000000004E-2</v>
       </c>
       <c r="G11">
-        <f t="shared" si="1"/>
-        <v>4.4000000000000011E-2</v>
+        <v>3.6000000000000004E-2</v>
       </c>
       <c r="H11">
-        <f t="shared" si="1"/>
-        <v>4.6000000000000013E-2</v>
+        <v>3.6000000000000004E-2</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12">
-        <v>6.4000000000000001E-2</v>
+        <v>4.9000000000000002E-2</v>
       </c>
       <c r="B12">
-        <f t="shared" si="1"/>
-        <v>6.6000000000000003E-2</v>
+        <v>4.9000000000000002E-2</v>
       </c>
       <c r="C12">
-        <f t="shared" si="1"/>
-        <v>6.8000000000000005E-2</v>
+        <v>4.9000000000000002E-2</v>
       </c>
       <c r="D12">
-        <f t="shared" si="1"/>
-        <v>7.0000000000000007E-2</v>
+        <v>4.9000000000000002E-2</v>
       </c>
       <c r="E12">
-        <f t="shared" si="1"/>
-        <v>7.2000000000000008E-2</v>
+        <v>4.9000000000000002E-2</v>
       </c>
       <c r="F12">
-        <f t="shared" si="1"/>
-        <v>7.400000000000001E-2</v>
+        <v>4.9000000000000002E-2</v>
       </c>
       <c r="G12">
-        <f t="shared" si="1"/>
-        <v>7.6000000000000012E-2</v>
+        <v>4.9000000000000002E-2</v>
       </c>
       <c r="H12">
-        <f t="shared" si="1"/>
-        <v>7.8000000000000014E-2</v>
+        <v>4.9000000000000002E-2</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13">
-        <v>0.128</v>
+        <v>6.4000000000000001E-2</v>
       </c>
       <c r="B13">
-        <f t="shared" si="1"/>
-        <v>0.13</v>
+        <v>6.4000000000000001E-2</v>
       </c>
       <c r="C13">
-        <f t="shared" si="1"/>
-        <v>0.13200000000000001</v>
+        <v>6.4000000000000001E-2</v>
       </c>
       <c r="D13">
-        <f t="shared" si="1"/>
-        <v>0.13400000000000001</v>
+        <v>6.4000000000000001E-2</v>
       </c>
       <c r="E13">
-        <f t="shared" si="1"/>
-        <v>0.13600000000000001</v>
+        <v>6.4000000000000001E-2</v>
       </c>
       <c r="F13">
-        <f t="shared" si="1"/>
-        <v>0.13800000000000001</v>
+        <v>6.4000000000000001E-2</v>
       </c>
       <c r="G13">
-        <f t="shared" si="1"/>
-        <v>0.14000000000000001</v>
+        <v>6.4000000000000001E-2</v>
       </c>
       <c r="H13">
-        <f t="shared" si="1"/>
-        <v>0.14200000000000002</v>
+        <v>6.4000000000000001E-2</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14">
-        <v>0.25600000000000001</v>
+        <v>0.2</v>
       </c>
       <c r="B14">
-        <f t="shared" si="1"/>
-        <v>0.25800000000000001</v>
+        <v>0.2</v>
       </c>
       <c r="C14">
-        <f t="shared" si="1"/>
-        <v>0.26</v>
+        <v>0.2</v>
       </c>
       <c r="D14">
-        <f t="shared" si="1"/>
-        <v>0.26200000000000001</v>
+        <v>0.2</v>
       </c>
       <c r="E14">
-        <f t="shared" si="1"/>
-        <v>0.26400000000000001</v>
+        <v>0.2</v>
       </c>
       <c r="F14">
-        <f t="shared" si="1"/>
-        <v>0.26600000000000001</v>
+        <v>0.2</v>
       </c>
       <c r="G14">
-        <f t="shared" si="1"/>
-        <v>0.26800000000000002</v>
+        <v>0.2</v>
       </c>
       <c r="H14">
-        <f t="shared" si="1"/>
-        <v>0.27</v>
+        <v>0.2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
I have no idea what else could be wrong but its lie there is too great of a response from the flight perfomance
</commit_message>
<xml_diff>
--- a/Aero design/Flight sim/hover stage sim - RK4 method/lookupTableCd.xlsx
+++ b/Aero design/Flight sim/hover stage sim - RK4 method/lookupTableCd.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joseph\Documents\Crash-Sat\Crash-Sat\Aero design\Flight sim\hover stage sim - RK4 method\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jhayes\Downloads\Crash-Sat-main\Crash-Sat-main\Aero design\Flight sim\hover stage sim - RK4 method\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83096A00-A8AB-4AB5-B438-DDFA2E5A1C14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B275546-EEC3-4F2A-B277-DD398C9334E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -351,17 +351,17 @@
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1:K14"/>
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1">
-        <v>1.6E-2</v>
+        <v>0.21600000000000003</v>
       </c>
       <c r="B1">
-        <v>1.6E-2</v>
+        <v>6.6000000000000003E-2</v>
       </c>
       <c r="C1">
         <v>1.6E-2</v>
@@ -382,12 +382,12 @@
         <v>1.6E-2</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>9.0000000000000011E-3</v>
+        <v>0.20900000000000002</v>
       </c>
       <c r="B2">
-        <v>9.0000000000000011E-3</v>
+        <v>5.9000000000000004E-2</v>
       </c>
       <c r="C2">
         <v>9.0000000000000011E-3</v>
@@ -408,12 +408,12 @@
         <v>9.0000000000000011E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>4.0000000000000001E-3</v>
+        <v>0.20400000000000001</v>
       </c>
       <c r="B3">
-        <v>4.0000000000000001E-3</v>
+        <v>5.4000000000000006E-2</v>
       </c>
       <c r="C3">
         <v>4.0000000000000001E-3</v>
@@ -434,12 +434,12 @@
         <v>4.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>1E-3</v>
+        <v>0.20100000000000001</v>
       </c>
       <c r="B4">
-        <v>1E-3</v>
+        <v>5.1000000000000004E-2</v>
       </c>
       <c r="C4">
         <v>1E-3</v>
@@ -460,12 +460,12 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -486,12 +486,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>1E-3</v>
+        <v>0.20100000000000001</v>
       </c>
       <c r="B6">
-        <v>1E-3</v>
+        <v>5.1000000000000004E-2</v>
       </c>
       <c r="C6">
         <v>1E-3</v>
@@ -512,12 +512,12 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>4.0000000000000001E-3</v>
+        <v>0.20400000000000001</v>
       </c>
       <c r="B7">
-        <v>4.0000000000000001E-3</v>
+        <v>5.4000000000000006E-2</v>
       </c>
       <c r="C7">
         <v>4.0000000000000001E-3</v>
@@ -538,12 +538,12 @@
         <v>4.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>9.0000000000000011E-3</v>
+        <v>0.20900000000000002</v>
       </c>
       <c r="B8">
-        <v>9.0000000000000011E-3</v>
+        <v>5.9000000000000004E-2</v>
       </c>
       <c r="C8">
         <v>9.0000000000000011E-3</v>
@@ -564,12 +564,12 @@
         <v>9.0000000000000011E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>1.6E-2</v>
+        <v>0.21600000000000003</v>
       </c>
       <c r="B9">
-        <v>1.6E-2</v>
+        <v>6.6000000000000003E-2</v>
       </c>
       <c r="C9">
         <v>1.6E-2</v>
@@ -590,12 +590,12 @@
         <v>1.6E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>2.5000000000000001E-2</v>
+        <v>0.22500000000000001</v>
       </c>
       <c r="B10">
-        <v>2.5000000000000001E-2</v>
+        <v>7.5000000000000011E-2</v>
       </c>
       <c r="C10">
         <v>2.5000000000000001E-2</v>
@@ -616,12 +616,12 @@
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>3.6000000000000004E-2</v>
+        <v>0.23600000000000002</v>
       </c>
       <c r="B11">
-        <v>3.6000000000000004E-2</v>
+        <v>8.6000000000000007E-2</v>
       </c>
       <c r="C11">
         <v>3.6000000000000004E-2</v>
@@ -642,12 +642,12 @@
         <v>3.6000000000000004E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>4.9000000000000002E-2</v>
+        <v>0.249</v>
       </c>
       <c r="B12">
-        <v>4.9000000000000002E-2</v>
+        <v>9.9000000000000005E-2</v>
       </c>
       <c r="C12">
         <v>4.9000000000000002E-2</v>
@@ -668,12 +668,12 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>6.4000000000000001E-2</v>
+        <v>0.26400000000000001</v>
       </c>
       <c r="B13">
-        <v>6.4000000000000001E-2</v>
+        <v>0.114</v>
       </c>
       <c r="C13">
         <v>6.4000000000000001E-2</v>
@@ -694,30 +694,30 @@
         <v>6.4000000000000001E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>0.2</v>
+        <v>0.7</v>
       </c>
       <c r="B14">
-        <v>0.2</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="C14">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="D14">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="E14">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="F14">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="G14">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="H14">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>